<commit_message>
Add Gernerate identify number fun
</commit_message>
<xml_diff>
--- a/CustomerReg/TestData/AccountReg.xlsx
+++ b/CustomerReg/TestData/AccountReg.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>客户类型</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -34,6 +34,14 @@
   </si>
   <si>
     <t>密码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qwe123</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>14412350000</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -77,8 +85,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -362,16 +371,19 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="15.375" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
@@ -382,9 +394,16 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>